<commit_message>
updated new entry in sheet
</commit_message>
<xml_diff>
--- a/SampleData/FullUserRegistration_org.xlsx
+++ b/SampleData/FullUserRegistration_org.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manbatra1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Manoj\Learning_01022022\manoj_utility\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B3870B-1847-4FE4-B9E0-25D108086732}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="404">
   <si>
     <t>Child</t>
   </si>
@@ -205,9 +206,6 @@
   </si>
   <si>
     <t>data.externalApplication.internalIdentifier</t>
-  </si>
-  <si>
-    <t>184021</t>
   </si>
   <si>
     <t>data.areaOfInterest.lastUpdateDate</t>
@@ -1232,12 +1230,21 @@
   </si>
   <si>
     <t>pl</t>
+  </si>
+  <si>
+    <t>184021565</t>
+  </si>
+  <si>
+    <t>'184021565</t>
+  </si>
+  <si>
+    <t>8402565</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -2469,168 +2476,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:KZ38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="GS1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="GZ7" sqref="GZ7"/>
+      <selection activeCell="GW3" sqref="GW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="12.42578125" style="6" customWidth="1"/>
-    <col min="9" max="10" width="19.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="12.453125" style="6" customWidth="1"/>
+    <col min="9" max="10" width="19.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.54296875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="37" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="37" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="39" max="45" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.7109375" style="6" customWidth="1"/>
+    <col min="46" max="46" width="17.7265625" style="6" customWidth="1"/>
     <col min="47" max="47" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="48" max="53" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="48" max="53" width="25.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="54" max="56" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="27.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="21.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="17.85546875" style="6" customWidth="1"/>
-    <col min="63" max="63" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="23.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="27.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="21.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="17.81640625" style="6" customWidth="1"/>
+    <col min="63" max="63" width="18.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="23.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="22" style="6" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.81640625" style="6" bestFit="1" customWidth="1"/>
     <col min="68" max="69" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="24.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="26" style="6" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="20.28515625" style="6" customWidth="1"/>
-    <col min="75" max="75" width="22.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="20.28515625" style="6" customWidth="1"/>
-    <col min="78" max="78" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="81" max="95" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="96" max="102" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="103" max="105" width="17.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="17.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="114" max="115" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="17.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="117" max="118" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="127" max="131" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="25.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="134" max="135" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="20.26953125" style="6" customWidth="1"/>
+    <col min="75" max="75" width="22.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="20.26953125" style="6" customWidth="1"/>
+    <col min="78" max="78" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="15.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="81" max="95" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="96" max="102" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="103" max="105" width="17.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="16.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="17.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="114" max="115" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="17.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="117" max="118" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="20.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="22.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="15.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="17.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="16.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="127" max="131" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="25.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="134" max="135" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="137" max="138" width="13" bestFit="1" customWidth="1"/>
     <col min="139" max="140" width="13" style="6" customWidth="1"/>
-    <col min="141" max="144" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="16.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="16.7109375" style="6" customWidth="1"/>
-    <col min="148" max="148" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="16.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="150" max="154" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="141" max="144" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="16.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="16.7265625" style="45" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="16.7265625" style="6" customWidth="1"/>
+    <col min="148" max="148" width="16.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="16.453125" style="45" bestFit="1" customWidth="1"/>
+    <col min="150" max="154" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="155" max="156" width="13" bestFit="1" customWidth="1"/>
     <col min="158" max="167" width="13" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="170" max="175" width="13.140625" style="6" customWidth="1"/>
-    <col min="176" max="176" width="13.140625" customWidth="1"/>
-    <col min="177" max="185" width="13.140625" style="6" customWidth="1"/>
-    <col min="186" max="187" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="188" max="189" width="13.140625" style="6" customWidth="1"/>
-    <col min="190" max="190" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="191" max="192" width="14.7109375" style="50" customWidth="1"/>
-    <col min="193" max="193" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="170" max="175" width="13.1796875" style="6" customWidth="1"/>
+    <col min="176" max="176" width="13.1796875" customWidth="1"/>
+    <col min="177" max="185" width="13.1796875" style="6" customWidth="1"/>
+    <col min="186" max="187" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="188" max="189" width="13.1796875" style="6" customWidth="1"/>
+    <col min="190" max="190" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="191" max="192" width="14.7265625" style="50" customWidth="1"/>
+    <col min="193" max="193" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="194" max="194" width="13" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="196" max="199" width="13" style="6" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="19.28515625" style="6" customWidth="1"/>
+    <col min="200" max="200" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="19.26953125" style="6" customWidth="1"/>
     <col min="202" max="207" width="13" style="6" customWidth="1"/>
-    <col min="208" max="208" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="209" max="210" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="213" max="218" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="33.140625" style="6" customWidth="1"/>
-    <col min="221" max="221" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="21.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="12.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="209" max="210" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="17.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="213" max="218" width="17.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="33.1796875" style="6" customWidth="1"/>
+    <col min="221" max="221" width="18.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="21.54296875" style="6" bestFit="1" customWidth="1"/>
     <col min="223" max="224" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="18.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="18.140625" style="6" customWidth="1"/>
+    <col min="225" max="225" width="32.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="18.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="18.1796875" style="6" customWidth="1"/>
     <col min="228" max="228" width="15" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="15" style="6" customWidth="1"/>
-    <col min="230" max="231" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="232" max="241" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="22.5703125" customWidth="1"/>
-    <col min="244" max="246" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="230" max="231" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="232" max="241" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="22.54296875" customWidth="1"/>
+    <col min="244" max="246" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="249" max="249" width="13" bestFit="1" customWidth="1"/>
-    <col min="250" max="251" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="250" max="251" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="252" max="252" width="13" bestFit="1" customWidth="1"/>
     <col min="253" max="258" width="13" style="6" customWidth="1"/>
     <col min="259" max="259" width="13" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="12.85546875" style="6" customWidth="1"/>
-    <col min="262" max="262" width="18.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="263" max="272" width="18.140625" style="6" customWidth="1"/>
-    <col min="273" max="273" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="274" max="278" width="18.140625" style="6" customWidth="1"/>
-    <col min="279" max="291" width="12.85546875" style="6" customWidth="1"/>
-    <col min="292" max="292" width="15.42578125" customWidth="1"/>
-    <col min="293" max="293" width="15.42578125" style="6" customWidth="1"/>
-    <col min="294" max="294" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="295" max="297" width="15.42578125" style="6" customWidth="1"/>
-    <col min="298" max="299" width="19.28515625" style="6" customWidth="1"/>
-    <col min="300" max="301" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="22.28515625" customWidth="1"/>
-    <col min="303" max="303" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="304" max="305" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="12.81640625" style="6" customWidth="1"/>
+    <col min="262" max="262" width="18.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="263" max="272" width="18.1796875" style="6" customWidth="1"/>
+    <col min="273" max="273" width="24.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="274" max="278" width="18.1796875" style="6" customWidth="1"/>
+    <col min="279" max="291" width="12.81640625" style="6" customWidth="1"/>
+    <col min="292" max="292" width="15.453125" customWidth="1"/>
+    <col min="293" max="293" width="15.453125" style="6" customWidth="1"/>
+    <col min="294" max="294" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="295" max="297" width="15.453125" style="6" customWidth="1"/>
+    <col min="298" max="299" width="19.26953125" style="6" customWidth="1"/>
+    <col min="300" max="301" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="22.26953125" customWidth="1"/>
+    <col min="303" max="303" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="304" max="305" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2692,7 +2699,7 @@
       <c r="GJ1" s="51"/>
       <c r="GR1" s="2"/>
       <c r="GT1" s="78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="GU1" s="78"/>
       <c r="GV1" s="78"/>
@@ -2704,7 +2711,7 @@
       <c r="HU1" s="4"/>
       <c r="II1" s="2"/>
       <c r="IR1" s="75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="IS1" s="76"/>
       <c r="IT1" s="76"/>
@@ -2754,18 +2761,18 @@
       <c r="KP1" s="73"/>
       <c r="KQ1" s="74"/>
       <c r="KR1" s="72" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="KS1" s="73"/>
       <c r="KT1" s="73"/>
       <c r="KU1" s="74"/>
     </row>
-    <row r="2" spans="1:312" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:312" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>3</v>
@@ -2774,28 +2781,28 @@
         <v>4</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="I2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="K2" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>385</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>386</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>54</v>
@@ -2807,367 +2814,367 @@
         <v>56</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="V2" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="W2" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="X2" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="Y2" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Z2" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="AA2" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AB2" s="15" t="s">
         <v>262</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>263</v>
       </c>
       <c r="AC2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="AD2" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE2" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AF2" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AG2" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AH2" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="AH2" s="15" t="s">
+      <c r="AI2" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="AI2" s="15" t="s">
+      <c r="AJ2" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="AJ2" s="15" t="s">
+      <c r="AK2" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>271</v>
       </c>
       <c r="AL2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="AM2" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN2" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="AN2" s="15" t="s">
+      <c r="AO2" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="AO2" s="15" t="s">
+      <c r="AP2" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="AP2" s="15" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AR2" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="AR2" s="15" t="s">
+      <c r="AS2" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="AS2" s="15" t="s">
+      <c r="AT2" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="AT2" s="15" t="s">
+      <c r="AU2" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="AU2" s="15" t="s">
+      <c r="AV2" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="AV2" s="15" t="s">
+      <c r="AW2" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="AW2" s="15" t="s">
+      <c r="AX2" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="AX2" s="15" t="s">
+      <c r="AY2" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="AY2" s="15" t="s">
+      <c r="AZ2" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="AZ2" s="15" t="s">
+      <c r="BA2" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="BA2" s="15" t="s">
+      <c r="BB2" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="BB2" s="15" t="s">
+      <c r="BC2" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="BC2" s="15" t="s">
+      <c r="BD2" s="15" t="s">
         <v>288</v>
-      </c>
-      <c r="BD2" s="15" t="s">
-        <v>289</v>
       </c>
       <c r="BE2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="BF2" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="BG2" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="BG2" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="BH2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="BI2" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="BJ2" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="BJ2" s="16" t="s">
+      <c r="BK2" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="BK2" s="16" t="s">
+      <c r="BL2" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="BL2" s="16" t="s">
+      <c r="BM2" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="BM2" s="16" t="s">
+      <c r="BN2" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="BN2" s="16" t="s">
+      <c r="BO2" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="BO2" s="16" t="s">
+      <c r="BP2" s="61" t="s">
         <v>298</v>
       </c>
-      <c r="BP2" s="61" t="s">
+      <c r="BQ2" s="61" t="s">
         <v>299</v>
       </c>
-      <c r="BQ2" s="61" t="s">
+      <c r="BR2" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="BR2" s="16" t="s">
+      <c r="BS2" s="16" t="s">
         <v>301</v>
-      </c>
-      <c r="BS2" s="16" t="s">
-        <v>302</v>
       </c>
       <c r="BT2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="BU2" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BV2" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BV2" s="15" t="s">
+      <c r="BW2" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="BW2" s="15" t="s">
+      <c r="BX2" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="BX2" s="15" t="s">
+      <c r="BY2" s="15" t="s">
         <v>306</v>
-      </c>
-      <c r="BY2" s="15" t="s">
-        <v>307</v>
       </c>
       <c r="BZ2" s="15" t="s">
         <v>45</v>
       </c>
       <c r="CA2" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="CB2" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="CB2" s="15" t="s">
+      <c r="CC2" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="CC2" s="3" t="s">
+      <c r="CD2" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="CD2" s="3" t="s">
+      <c r="CE2" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="CE2" s="3" t="s">
+      <c r="CF2" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="CF2" s="3" t="s">
+      <c r="CG2" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="CG2" s="3" t="s">
+      <c r="CH2" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="CH2" s="3" t="s">
+      <c r="CI2" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="CI2" s="15" t="s">
+      <c r="CJ2" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="CJ2" s="15" t="s">
+      <c r="CK2" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="CK2" s="15" t="s">
+      <c r="CL2" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="CL2" s="15" t="s">
+      <c r="CM2" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="CM2" s="15" t="s">
+      <c r="CN2" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="CN2" s="15" t="s">
+      <c r="CO2" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="CO2" s="15" t="s">
+      <c r="CP2" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="CP2" s="15" t="s">
+      <c r="CQ2" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="CQ2" s="15" t="s">
+      <c r="CR2" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="CR2" s="15" t="s">
+      <c r="CS2" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="CS2" s="15" t="s">
+      <c r="CT2" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="CT2" s="15" t="s">
+      <c r="CU2" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="CU2" s="15" t="s">
+      <c r="CV2" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="CV2" s="15" t="s">
+      <c r="CW2" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="CW2" s="15" t="s">
+      <c r="CX2" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="CX2" s="15" t="s">
+      <c r="CY2" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="CY2" s="15" t="s">
+      <c r="CZ2" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="CZ2" s="15" t="s">
+      <c r="DA2" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="DA2" s="15" t="s">
+      <c r="DB2" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="DB2" s="15" t="s">
+      <c r="DC2" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="DC2" s="15" t="s">
+      <c r="DD2" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="DD2" s="15" t="s">
+      <c r="DE2" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="DE2" s="15" t="s">
+      <c r="DF2" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="DF2" s="15" t="s">
+      <c r="DG2" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="DG2" s="15" t="s">
+      <c r="DH2" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="DH2" s="15" t="s">
+      <c r="DI2" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="DI2" s="15" t="s">
+      <c r="DJ2" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="DJ2" s="15" t="s">
+      <c r="DK2" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="DK2" s="15" t="s">
+      <c r="DL2" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="DL2" s="15" t="s">
+      <c r="DM2" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="DM2" s="15" t="s">
+      <c r="DN2" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="DN2" s="15" t="s">
+      <c r="DO2" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="DO2" s="15" t="s">
+      <c r="DP2" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="DP2" s="15" t="s">
+      <c r="DQ2" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="DQ2" s="15" t="s">
+      <c r="DR2" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="DR2" s="15" t="s">
+      <c r="DS2" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="DS2" s="15" t="s">
+      <c r="DT2" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="DT2" s="15" t="s">
+      <c r="DU2" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="DU2" s="15" t="s">
+      <c r="DV2" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="DV2" s="15" t="s">
+      <c r="DW2" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="DW2" s="15" t="s">
+      <c r="DX2" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="DX2" s="15" t="s">
+      <c r="DY2" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="DY2" s="15" t="s">
+      <c r="DZ2" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="DZ2" s="15" t="s">
+      <c r="EA2" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="EA2" s="15" t="s">
+      <c r="EB2" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="EB2" s="15" t="s">
+      <c r="EC2" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="EC2" s="15" t="s">
+      <c r="ED2" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="ED2" s="15" t="s">
+      <c r="EE2" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="EE2" s="15" t="s">
+      <c r="EF2" s="15" t="s">
         <v>364</v>
-      </c>
-      <c r="EF2" s="15" t="s">
-        <v>365</v>
       </c>
       <c r="EG2" s="15" t="s">
         <v>15</v>
@@ -3176,10 +3183,10 @@
         <v>22</v>
       </c>
       <c r="EI2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="EJ2" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="EJ2" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="EK2" s="15" t="s">
         <v>10</v>
@@ -3200,67 +3207,67 @@
         <v>42</v>
       </c>
       <c r="EQ2" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="ER2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="ES2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="ET2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="EU2" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="EU2" s="3" t="s">
+      <c r="EV2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="EV2" s="3" t="s">
+      <c r="EW2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="EW2" s="3" t="s">
+      <c r="EX2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="EX2" s="3" t="s">
+      <c r="EY2" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="EY2" s="15" t="s">
+      <c r="EZ2" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="EZ2" s="15" t="s">
+      <c r="FA2" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="FA2" s="15" t="s">
+      <c r="FB2" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="FB2" s="15" t="s">
+      <c r="FC2" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="FC2" s="15" t="s">
+      <c r="FD2" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="FD2" s="15" t="s">
+      <c r="FE2" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="FE2" s="15" t="s">
+      <c r="FF2" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="FF2" s="15" t="s">
+      <c r="FG2" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="FG2" s="15" t="s">
+      <c r="FH2" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="FH2" s="15" t="s">
+      <c r="FI2" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="FI2" s="15" t="s">
+      <c r="FJ2" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="FJ2" s="15" t="s">
+      <c r="FK2" s="15" t="s">
         <v>191</v>
-      </c>
-      <c r="FK2" s="15" t="s">
-        <v>192</v>
       </c>
       <c r="FL2" s="15" t="s">
         <v>16</v>
@@ -3269,22 +3276,22 @@
         <v>17</v>
       </c>
       <c r="FN2" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="FO2" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="FO2" s="13" t="s">
+      <c r="FP2" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="FP2" s="13" t="s">
+      <c r="FQ2" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="FQ2" s="13" t="s">
+      <c r="FR2" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="FR2" s="13" t="s">
-        <v>372</v>
-      </c>
       <c r="FS2" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="FT2" s="13" t="s">
         <v>26</v>
@@ -3293,40 +3300,40 @@
         <v>28</v>
       </c>
       <c r="FV2" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="FW2" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="FX2" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="FY2" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="FZ2" s="13" t="s">
         <v>208</v>
-      </c>
-      <c r="FW2" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="FX2" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="FY2" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="FZ2" s="13" t="s">
-        <v>209</v>
       </c>
       <c r="GA2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="GB2" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="GC2" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="GC2" s="13" t="s">
+      <c r="GD2" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="GD2" s="13" t="s">
+      <c r="GE2" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="GE2" s="13" t="s">
+      <c r="GF2" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="GF2" s="13" t="s">
+      <c r="GG2" s="13" t="s">
         <v>214</v>
-      </c>
-      <c r="GG2" s="13" t="s">
-        <v>215</v>
       </c>
       <c r="GH2" s="13" t="s">
         <v>29</v>
@@ -3335,328 +3342,328 @@
         <v>25</v>
       </c>
       <c r="GJ2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="GK2" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="GL2" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="GM2" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="GN2" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="GK2" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="GL2" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="GM2" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="GN2" s="46" t="s">
+      <c r="GO2" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="GO2" s="46" t="s">
+      <c r="GP2" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="GP2" s="46" t="s">
+      <c r="GQ2" s="46" t="s">
         <v>219</v>
-      </c>
-      <c r="GQ2" s="46" t="s">
-        <v>220</v>
       </c>
       <c r="GR2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="GS2" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="GT2" s="34" t="s">
         <v>58</v>
       </c>
       <c r="GU2" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="GV2" s="34" t="s">
         <v>222</v>
-      </c>
-      <c r="GV2" s="34" t="s">
-        <v>223</v>
       </c>
       <c r="GW2" s="34" t="s">
         <v>59</v>
       </c>
       <c r="GX2" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="GY2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="GY2" s="3" t="s">
+      <c r="GZ2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="HA2" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="GZ2" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="HA2" s="3" t="s">
+      <c r="HB2" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="HB2" s="3" t="s">
+      <c r="HC2" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="HC2" s="3" t="s">
+      <c r="HD2" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="HD2" s="3" t="s">
+      <c r="HE2" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="HE2" s="3" t="s">
+      <c r="HF2" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="HF2" s="3" t="s">
+      <c r="HG2" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="HG2" s="3" t="s">
+      <c r="HH2" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="HH2" s="3" t="s">
+      <c r="HI2" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="HI2" s="3" t="s">
+      <c r="HJ2" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="HJ2" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="HK2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="HL2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="HM2" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="HM2" s="3" t="s">
+      <c r="HN2" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="HN2" s="3" t="s">
+      <c r="HO2" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="HO2" s="3" t="s">
+      <c r="HP2" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="HP2" s="3" t="s">
+      <c r="HQ2" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="HQ2" s="3" t="s">
+      <c r="HR2" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="HR2" s="3" t="s">
+      <c r="HS2" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="HS2" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="HT2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="HU2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="HV2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="HW2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="HX2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="HY2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="HZ2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="IA2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="IB2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="IC2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="ID2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="IE2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="IF2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="IG2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="IH2" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="HV2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="HW2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="HX2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="HY2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="HZ2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="IA2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="IB2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="IC2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="ID2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="IE2" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="IF2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="IG2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="IH2" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="II2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="IJ2" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="IK2" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="IK2" s="46" t="s">
+      <c r="IL2" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="IL2" s="46" t="s">
+      <c r="IM2" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="IM2" s="46" t="s">
+      <c r="IN2" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="IN2" s="46" t="s">
+      <c r="IO2" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="IO2" s="46" t="s">
+      <c r="IP2" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="IP2" s="46" t="s">
+      <c r="IQ2" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="IQ2" s="46" t="s">
-        <v>203</v>
-      </c>
       <c r="IR2" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="IS2" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="IT2" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="IU2" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="IV2" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="IW2" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="IX2" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="IY2" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="IZ2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="JA2" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="JB2" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="JC2" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="JD2" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="JE2" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="JF2" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="JG2" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="JH2" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="JI2" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="JJ2" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="JK2" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="JL2" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="JM2" s="38" t="s">
+        <v>389</v>
+      </c>
+      <c r="JN2" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="JO2" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="JP2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="JQ2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="IS2" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="IT2" s="38" t="s">
-        <v>376</v>
-      </c>
-      <c r="IU2" s="38" t="s">
-        <v>377</v>
-      </c>
-      <c r="IV2" s="38" t="s">
-        <v>378</v>
-      </c>
-      <c r="IW2" s="38" t="s">
-        <v>379</v>
-      </c>
-      <c r="IX2" s="38" t="s">
-        <v>380</v>
-      </c>
-      <c r="IY2" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="IZ2" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="JA2" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="JB2" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="JC2" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="JD2" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="JE2" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="JF2" s="38" t="s">
-        <v>382</v>
-      </c>
-      <c r="JG2" s="38" t="s">
-        <v>383</v>
-      </c>
-      <c r="JH2" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="JI2" s="38" t="s">
+      <c r="JR2" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="JS2" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="JJ2" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="JK2" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="JL2" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="JM2" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="JN2" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="JO2" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="JP2" s="38" t="s">
+      <c r="JT2" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="JQ2" s="38" t="s">
+      <c r="JU2" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="JV2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="JW2" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="JX2" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="JY2" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="JZ2" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="KA2" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="KB2" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="KC2" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="KD2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="JR2" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="JS2" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="JT2" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="JU2" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="JV2" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="JW2" s="59" t="s">
-        <v>246</v>
-      </c>
-      <c r="JX2" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="JY2" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="JZ2" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="KA2" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="KB2" s="38" t="s">
+      <c r="KE2" s="38" t="s">
         <v>146</v>
-      </c>
-      <c r="KC2" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="KD2" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="KE2" s="38" t="s">
-        <v>147</v>
       </c>
       <c r="KF2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="KG2" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="KH2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="KI2" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="KJ2" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="KJ2" s="3" t="s">
+      <c r="KK2" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="KK2" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="KL2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="KM2" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="KN2" s="14" t="s">
         <v>35</v>
@@ -3671,24 +3678,24 @@
         <v>38</v>
       </c>
       <c r="KR2" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="KS2" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="KS2" s="14" t="s">
+      <c r="KT2" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="KT2" s="14" t="s">
+      <c r="KU2" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="KU2" s="14" t="s">
-        <v>398</v>
-      </c>
     </row>
-    <row r="3" spans="1:312" s="33" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:312" s="33" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="7" t="b">
         <v>1</v>
@@ -3710,10 +3717,10 @@
         <v>39</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="30"/>
@@ -3792,7 +3799,7 @@
       <c r="BX3" s="24"/>
       <c r="BY3" s="24"/>
       <c r="BZ3" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA3" s="24"/>
       <c r="CB3" s="24"/>
@@ -3870,14 +3877,14 @@
         <v>44</v>
       </c>
       <c r="EP3" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="EQ3" s="21"/>
       <c r="ER3" s="17" t="s">
         <v>43</v>
       </c>
       <c r="ES3" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="ET3" s="66"/>
       <c r="EU3" s="66"/>
@@ -3901,7 +3908,7 @@
         <v>37682</v>
       </c>
       <c r="FM3" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FN3" s="67"/>
       <c r="FO3" s="68"/>
@@ -3913,7 +3920,7 @@
         <v>41335</v>
       </c>
       <c r="FU3" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FV3" s="25"/>
       <c r="FW3" s="71"/>
@@ -3921,7 +3928,7 @@
       <c r="FY3" s="71"/>
       <c r="FZ3" s="25"/>
       <c r="GA3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="GB3" s="25"/>
       <c r="GC3" s="25"/>
@@ -3944,12 +3951,12 @@
       <c r="GR3" s="24"/>
       <c r="GS3" s="24"/>
       <c r="GT3" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="GU3" s="27"/>
       <c r="GV3" s="27"/>
       <c r="GW3" s="28" t="s">
-        <v>60</v>
+        <v>401</v>
       </c>
       <c r="GX3" s="28"/>
       <c r="GY3" s="53"/>
@@ -3967,7 +3974,7 @@
       <c r="HI3" s="24"/>
       <c r="HJ3" s="24"/>
       <c r="HK3" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HL3" s="26"/>
       <c r="HM3" s="26"/>
@@ -3985,25 +3992,25 @@
         <v>1</v>
       </c>
       <c r="HW3" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="HX3" s="32" t="b">
         <v>1</v>
       </c>
       <c r="HY3" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="HZ3" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="IA3" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="IB3" s="32" t="b">
         <v>1</v>
       </c>
       <c r="IC3" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="ID3" s="32"/>
       <c r="IE3" s="32"/>
@@ -4036,7 +4043,7 @@
       </c>
       <c r="JA3" s="40"/>
       <c r="JB3" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC3" s="43" t="b">
         <v>0</v>
@@ -4048,7 +4055,7 @@
       <c r="JF3" s="63"/>
       <c r="JG3" s="63"/>
       <c r="JH3" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JI3" s="43" t="b">
         <v>0</v>
@@ -4063,10 +4070,10 @@
         <v>0</v>
       </c>
       <c r="JM3" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JN3" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="JO3" s="43" t="b">
         <v>0</v>
@@ -4075,13 +4082,13 @@
         <v>0</v>
       </c>
       <c r="JQ3" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="JR3" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="JS3" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="JT3" s="25" t="b">
         <v>1</v>
@@ -4112,33 +4119,33 @@
       <c r="KL3" s="24"/>
       <c r="KM3" s="24"/>
       <c r="KN3" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="KO3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KP3" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="KQ3" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR3" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="KS3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KT3" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="KU3" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:312" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:312" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="7" t="b">
@@ -4158,25 +4165,25 @@
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N4" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="32"/>
@@ -4251,7 +4258,7 @@
       <c r="BX4" s="24"/>
       <c r="BY4" s="24"/>
       <c r="BZ4" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA4" s="24"/>
       <c r="CB4" s="24"/>
@@ -4312,7 +4319,7 @@
       <c r="EE4" s="24"/>
       <c r="EF4" s="24"/>
       <c r="EG4" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="EH4" s="7"/>
       <c r="EI4" s="7"/>
@@ -4329,14 +4336,14 @@
         <v>123456</v>
       </c>
       <c r="EP4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="EQ4" s="21"/>
       <c r="ER4" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="ES4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="ET4" s="63"/>
       <c r="EU4" s="63"/>
@@ -4360,7 +4367,7 @@
         <v>37683</v>
       </c>
       <c r="FM4" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FN4" s="67"/>
       <c r="FO4" s="68"/>
@@ -4372,7 +4379,7 @@
         <v>41335</v>
       </c>
       <c r="FU4" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FV4" s="25"/>
       <c r="FW4" s="71"/>
@@ -4380,7 +4387,7 @@
       <c r="FY4" s="71"/>
       <c r="FZ4" s="25"/>
       <c r="GA4" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="GB4" s="25"/>
       <c r="GC4" s="25"/>
@@ -4389,7 +4396,7 @@
       <c r="GF4" s="43"/>
       <c r="GG4" s="43"/>
       <c r="GH4" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="GI4" s="48"/>
       <c r="GJ4" s="48"/>
@@ -4422,7 +4429,7 @@
       <c r="HI4" s="24"/>
       <c r="HJ4" s="24"/>
       <c r="HK4" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HL4" s="26"/>
       <c r="HM4" s="26"/>
@@ -4433,32 +4440,32 @@
       <c r="HR4" s="26"/>
       <c r="HS4" s="26"/>
       <c r="HT4" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="HU4" s="25"/>
       <c r="HV4" s="32" t="b">
         <v>1</v>
       </c>
       <c r="HW4" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="HX4" s="32" t="b">
         <v>1</v>
       </c>
       <c r="HY4" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="HZ4" s="54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="IA4" s="54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="IB4" s="55" t="b">
         <v>1</v>
       </c>
       <c r="IC4" s="56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="ID4" s="43"/>
       <c r="IE4" s="43"/>
@@ -4491,7 +4498,7 @@
       </c>
       <c r="JA4" s="40"/>
       <c r="JB4" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC4" s="43" t="b">
         <v>0</v>
@@ -4503,7 +4510,7 @@
       <c r="JF4" s="63"/>
       <c r="JG4" s="63"/>
       <c r="JH4" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JI4" s="43" t="b">
         <v>0</v>
@@ -4518,10 +4525,10 @@
         <v>0</v>
       </c>
       <c r="JM4" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JN4" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="JO4" s="43" t="b">
         <v>0</v>
@@ -4530,13 +4537,13 @@
         <v>0</v>
       </c>
       <c r="JQ4" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="JR4" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="JS4" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="JT4" s="25" t="b">
         <v>1</v>
@@ -4567,16 +4574,16 @@
       <c r="KL4" s="24"/>
       <c r="KM4" s="24"/>
       <c r="KN4" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="KO4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KP4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="KQ4" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR4" s="15"/>
       <c r="KS4" s="7"/>
@@ -4584,9 +4591,9 @@
       <c r="KU4" s="7"/>
       <c r="KZ4" s="33"/>
     </row>
-    <row r="5" spans="1:312" ht="54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:312" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="7" t="b">
@@ -4608,19 +4615,19 @@
       <c r="I5" s="19"/>
       <c r="J5" s="20"/>
       <c r="K5" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O5" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="32"/>
@@ -4695,7 +4702,7 @@
       <c r="BX5" s="24"/>
       <c r="BY5" s="24"/>
       <c r="BZ5" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA5" s="24"/>
       <c r="CB5" s="24"/>
@@ -4756,13 +4763,13 @@
       <c r="EE5" s="24"/>
       <c r="EF5" s="24"/>
       <c r="EG5" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="EH5" s="7"/>
       <c r="EI5" s="7"/>
       <c r="EJ5" s="7"/>
       <c r="EK5" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="EL5" s="24" t="s">
         <v>52</v>
@@ -4796,7 +4803,7 @@
         <v>37683</v>
       </c>
       <c r="FM5" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FN5" s="67"/>
       <c r="FO5" s="68"/>
@@ -4852,7 +4859,7 @@
       <c r="HI5" s="24"/>
       <c r="HJ5" s="24"/>
       <c r="HK5" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HL5" s="26"/>
       <c r="HM5" s="26"/>
@@ -4937,28 +4944,28 @@
       <c r="KL5" s="24"/>
       <c r="KM5" s="24"/>
       <c r="KN5" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="KO5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KP5" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="KQ5" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR5" s="15"/>
       <c r="KS5" s="7"/>
       <c r="KT5" s="22"/>
       <c r="KU5" s="7"/>
     </row>
-    <row r="6" spans="1:312" ht="81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:312" ht="78.5" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C6" s="7" t="b">
         <v>1</v>
@@ -4970,31 +4977,31 @@
         <v>1</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N6" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O6" s="31"/>
       <c r="P6" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q6" s="32"/>
       <c r="R6" s="23"/>
@@ -5009,7 +5016,7 @@
       <c r="AA6" s="23"/>
       <c r="AB6" s="23"/>
       <c r="AC6" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AD6" s="23"/>
       <c r="AE6" s="23"/>
@@ -5020,7 +5027,7 @@
       <c r="AJ6" s="23"/>
       <c r="AK6" s="23"/>
       <c r="AL6" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM6" s="23"/>
       <c r="AN6" s="23"/>
@@ -5041,12 +5048,12 @@
       <c r="BC6" s="23"/>
       <c r="BD6" s="23"/>
       <c r="BE6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BF6" s="7"/>
       <c r="BG6" s="7"/>
       <c r="BH6" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BI6" s="19"/>
       <c r="BJ6" s="19"/>
@@ -5060,7 +5067,7 @@
       <c r="BR6" s="19"/>
       <c r="BS6" s="19"/>
       <c r="BT6" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BU6" s="24"/>
       <c r="BV6" s="24"/>
@@ -5068,7 +5075,7 @@
       <c r="BX6" s="24"/>
       <c r="BY6" s="24"/>
       <c r="BZ6" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA6" s="24"/>
       <c r="CB6" s="24"/>
@@ -5129,16 +5136,16 @@
       <c r="EE6" s="24"/>
       <c r="EF6" s="24"/>
       <c r="EG6" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="EH6" s="7"/>
       <c r="EI6" s="7"/>
       <c r="EJ6" s="7"/>
       <c r="EK6" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="EL6" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="EM6" s="24"/>
       <c r="EN6" s="24"/>
@@ -5146,14 +5153,14 @@
         <v>44</v>
       </c>
       <c r="EP6" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="EQ6" s="21"/>
       <c r="ER6" s="17" t="s">
         <v>43</v>
       </c>
       <c r="ES6" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="ET6" s="63"/>
       <c r="EU6" s="63"/>
@@ -5177,7 +5184,7 @@
         <v>37683</v>
       </c>
       <c r="FM6" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FN6" s="70"/>
       <c r="FO6" s="70"/>
@@ -5212,12 +5219,12 @@
       <c r="GR6" s="24"/>
       <c r="GS6" s="24"/>
       <c r="GT6" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="GU6" s="27"/>
       <c r="GV6" s="27"/>
       <c r="GW6" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="GX6" s="28"/>
       <c r="GY6" s="53"/>
@@ -5237,7 +5244,7 @@
       <c r="HI6" s="24"/>
       <c r="HJ6" s="24"/>
       <c r="HK6" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HL6" s="26"/>
       <c r="HM6" s="26"/>
@@ -5248,7 +5255,7 @@
       <c r="HR6" s="26"/>
       <c r="HS6" s="26"/>
       <c r="HT6" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="HU6" s="25"/>
       <c r="HV6" s="43"/>
@@ -5316,7 +5323,7 @@
       <c r="KF6" s="25"/>
       <c r="KG6" s="25"/>
       <c r="KH6" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="KI6" s="25"/>
       <c r="KJ6" s="25"/>
@@ -5324,28 +5331,28 @@
       <c r="KL6" s="24"/>
       <c r="KM6" s="24"/>
       <c r="KN6" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="KO6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KP6" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="KQ6" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR6" s="43"/>
       <c r="KS6" s="43"/>
       <c r="KT6" s="43"/>
       <c r="KU6" s="43"/>
     </row>
-    <row r="7" spans="1:312" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:312" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C7" s="7" t="b">
         <v>1</v>
@@ -5357,30 +5364,30 @@
         <v>1</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="32"/>
@@ -5396,7 +5403,7 @@
       <c r="AA7" s="23"/>
       <c r="AB7" s="23"/>
       <c r="AC7" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AD7" s="23"/>
       <c r="AE7" s="23"/>
@@ -5407,7 +5414,7 @@
       <c r="AJ7" s="23"/>
       <c r="AK7" s="23"/>
       <c r="AL7" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AM7" s="23"/>
       <c r="AN7" s="23"/>
@@ -5428,7 +5435,7 @@
       <c r="BC7" s="23"/>
       <c r="BD7" s="23"/>
       <c r="BE7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BF7" s="7"/>
       <c r="BG7" s="7"/>
@@ -5447,7 +5454,7 @@
       <c r="BR7" s="19"/>
       <c r="BS7" s="43"/>
       <c r="BT7" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BU7" s="24"/>
       <c r="BV7" s="24"/>
@@ -5455,7 +5462,7 @@
       <c r="BX7" s="23"/>
       <c r="BY7" s="24"/>
       <c r="BZ7" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA7" s="24"/>
       <c r="CB7" s="24"/>
@@ -5516,13 +5523,13 @@
       <c r="EE7" s="24"/>
       <c r="EF7" s="24"/>
       <c r="EG7" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="EH7" s="7"/>
       <c r="EI7" s="7"/>
       <c r="EJ7" s="7"/>
       <c r="EK7" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="EL7" s="24">
         <v>1234</v>
@@ -5533,7 +5540,7 @@
         <v>44</v>
       </c>
       <c r="EP7" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="EQ7" s="21" t="b">
         <v>1</v>
@@ -5542,7 +5549,7 @@
         <v>43</v>
       </c>
       <c r="ES7" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="ET7" s="63"/>
       <c r="EU7" s="63"/>
@@ -5566,7 +5573,7 @@
         <v>37683</v>
       </c>
       <c r="FM7" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="FN7" s="67"/>
       <c r="FO7" s="68"/>
@@ -5578,7 +5585,7 @@
         <v>43526</v>
       </c>
       <c r="FU7" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="FV7" s="25"/>
       <c r="FW7" s="71"/>
@@ -5586,7 +5593,7 @@
       <c r="FY7" s="71"/>
       <c r="FZ7" s="25"/>
       <c r="GA7" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="GB7" s="25"/>
       <c r="GC7" s="25"/>
@@ -5595,7 +5602,7 @@
       <c r="GF7" s="43"/>
       <c r="GG7" s="43"/>
       <c r="GH7" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="GI7" s="48"/>
       <c r="GJ7" s="48"/>
@@ -5609,12 +5616,12 @@
       <c r="GR7" s="24"/>
       <c r="GS7" s="24"/>
       <c r="GT7" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="GU7" s="27"/>
       <c r="GV7" s="27"/>
       <c r="GW7" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="GX7" s="28"/>
       <c r="GY7" s="53"/>
@@ -5634,7 +5641,7 @@
       <c r="HI7" s="24"/>
       <c r="HJ7" s="24"/>
       <c r="HK7" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HL7" s="26"/>
       <c r="HM7" s="26"/>
@@ -5645,22 +5652,22 @@
       <c r="HR7" s="26"/>
       <c r="HS7" s="26"/>
       <c r="HT7" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="HU7" s="25"/>
       <c r="HV7" s="32" t="b">
         <v>1</v>
       </c>
       <c r="HW7" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="HX7" s="32"/>
       <c r="HY7" s="32"/>
       <c r="HZ7" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="IA7" s="57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="IB7" s="58"/>
       <c r="IC7" s="58"/>
@@ -5695,7 +5702,7 @@
       </c>
       <c r="JA7" s="40"/>
       <c r="JB7" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC7" s="43" t="b">
         <v>0</v>
@@ -5707,7 +5714,7 @@
       <c r="JF7" s="63"/>
       <c r="JG7" s="63"/>
       <c r="JH7" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JI7" s="43" t="b">
         <v>0</v>
@@ -5722,10 +5729,10 @@
         <v>0</v>
       </c>
       <c r="JM7" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JN7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="JO7" s="43" t="b">
         <v>0</v>
@@ -5734,13 +5741,13 @@
         <v>0</v>
       </c>
       <c r="JQ7" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="JR7" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="JS7" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="JT7" s="25" t="b">
         <v>1</v>
@@ -5763,7 +5770,7 @@
       <c r="KF7" s="25"/>
       <c r="KG7" s="25"/>
       <c r="KH7" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="KI7" s="25"/>
       <c r="KJ7" s="25"/>
@@ -5771,31 +5778,31 @@
       <c r="KL7" s="24"/>
       <c r="KM7" s="24"/>
       <c r="KN7" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="KO7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KP7" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="KQ7" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR7" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="KS7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="KT7" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="KU7" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -6045,7 +6052,7 @@
       <c r="KL8" s="1"/>
       <c r="KM8" s="1"/>
     </row>
-    <row r="9" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -6293,7 +6300,7 @@
       <c r="KL9" s="1"/>
       <c r="KM9" s="1"/>
     </row>
-    <row r="10" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6541,7 +6548,7 @@
       <c r="KL10" s="1"/>
       <c r="KM10" s="1"/>
     </row>
-    <row r="11" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -6789,7 +6796,7 @@
       <c r="KL11" s="1"/>
       <c r="KM11" s="1"/>
     </row>
-    <row r="12" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -7037,7 +7044,7 @@
       <c r="KL12" s="1"/>
       <c r="KM12" s="1"/>
     </row>
-    <row r="13" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -7285,7 +7292,7 @@
       <c r="KL13" s="1"/>
       <c r="KM13" s="1"/>
     </row>
-    <row r="14" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -7533,7 +7540,7 @@
       <c r="KL14" s="1"/>
       <c r="KM14" s="1"/>
     </row>
-    <row r="15" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7781,7 +7788,7 @@
       <c r="KL15" s="1"/>
       <c r="KM15" s="1"/>
     </row>
-    <row r="16" spans="1:312" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:312" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -8029,7 +8036,7 @@
       <c r="KL16" s="1"/>
       <c r="KM16" s="1"/>
     </row>
-    <row r="17" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -8277,7 +8284,7 @@
       <c r="KL17" s="1"/>
       <c r="KM17" s="1"/>
     </row>
-    <row r="18" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -8525,7 +8532,7 @@
       <c r="KL18" s="1"/>
       <c r="KM18" s="1"/>
     </row>
-    <row r="19" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -8773,7 +8780,7 @@
       <c r="KL19" s="1"/>
       <c r="KM19" s="1"/>
     </row>
-    <row r="20" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -9021,7 +9028,7 @@
       <c r="KL20" s="1"/>
       <c r="KM20" s="1"/>
     </row>
-    <row r="21" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -9269,7 +9276,7 @@
       <c r="KL21" s="1"/>
       <c r="KM21" s="1"/>
     </row>
-    <row r="22" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -9517,7 +9524,7 @@
       <c r="KL22" s="1"/>
       <c r="KM22" s="1"/>
     </row>
-    <row r="23" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -9765,7 +9772,7 @@
       <c r="KL23" s="1"/>
       <c r="KM23" s="1"/>
     </row>
-    <row r="24" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -10013,7 +10020,7 @@
       <c r="KL24" s="1"/>
       <c r="KM24" s="1"/>
     </row>
-    <row r="25" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -10261,7 +10268,7 @@
       <c r="KL25" s="1"/>
       <c r="KM25" s="1"/>
     </row>
-    <row r="26" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -10509,7 +10516,7 @@
       <c r="KL26" s="1"/>
       <c r="KM26" s="1"/>
     </row>
-    <row r="27" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -10757,7 +10764,7 @@
       <c r="KL27" s="1"/>
       <c r="KM27" s="1"/>
     </row>
-    <row r="28" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -11005,7 +11012,7 @@
       <c r="KL28" s="1"/>
       <c r="KM28" s="1"/>
     </row>
-    <row r="29" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -11253,7 +11260,7 @@
       <c r="KL29" s="1"/>
       <c r="KM29" s="1"/>
     </row>
-    <row r="30" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -11501,7 +11508,7 @@
       <c r="KL30" s="1"/>
       <c r="KM30" s="1"/>
     </row>
-    <row r="31" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -11749,7 +11756,7 @@
       <c r="KL31" s="1"/>
       <c r="KM31" s="1"/>
     </row>
-    <row r="32" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -11997,7 +12004,7 @@
       <c r="KL32" s="1"/>
       <c r="KM32" s="1"/>
     </row>
-    <row r="33" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -12245,7 +12252,7 @@
       <c r="KL33" s="1"/>
       <c r="KM33" s="1"/>
     </row>
-    <row r="34" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -12493,7 +12500,7 @@
       <c r="KL34" s="1"/>
       <c r="KM34" s="1"/>
     </row>
-    <row r="35" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -12741,7 +12748,7 @@
       <c r="KL35" s="1"/>
       <c r="KM35" s="1"/>
     </row>
-    <row r="36" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -12989,7 +12996,7 @@
       <c r="KL36" s="1"/>
       <c r="KM36" s="1"/>
     </row>
-    <row r="37" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -13237,7 +13244,7 @@
       <c r="KL37" s="1"/>
       <c r="KM37" s="1"/>
     </row>
-    <row r="38" spans="1:299" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -13494,20 +13501,20 @@
     <mergeCell ref="KR1:KU1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="AL5" r:id="rId3"/>
-    <hyperlink ref="AL4" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="G4:G5" r:id="rId6" display="zkhan@yopmail.com"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="G6" r:id="rId8"/>
-    <hyperlink ref="AL3" r:id="rId9"/>
-    <hyperlink ref="F5" r:id="rId10"/>
-    <hyperlink ref="F6" r:id="rId11"/>
-    <hyperlink ref="F7" r:id="rId12"/>
-    <hyperlink ref="AL6" r:id="rId13"/>
-    <hyperlink ref="AL7" r:id="rId14"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AL5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AL4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G4:G5" r:id="rId6" display="zkhan@yopmail.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AL3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AL6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AL7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId15"/>
@@ -13518,21 +13525,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
@@ -13543,18 +13550,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>

</xml_diff>